<commit_message>
Adding marshal data builder.
</commit_message>
<xml_diff>
--- a/data/Sample Rally.xlsx
+++ b/data/Sample Rally.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\round-table-car-rally\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB94DA3E-BCC2-4209-8E29-2F11E84CB4B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC375DB-4084-4051-8275-8BFDAF0BDEBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{83D86452-F20F-44D9-8BE9-A750E33F13C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{83D86452-F20F-44D9-8BE9-A750E33F13C5}"/>
   </bookViews>
   <sheets>
     <sheet name="CarRally23" sheetId="1" r:id="rId1"/>
@@ -287,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -308,6 +308,12 @@
     <xf numFmtId="21" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="21" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -317,13 +323,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="21" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,24 +639,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A2BD83-87CC-4D86-B37D-1F1B84049F58}">
   <dimension ref="A1:O381"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="94" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="16384" width="9.140625" style="26"/>
+    <col min="12" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="28"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6" t="s">
         <v>5</v>
@@ -1324,7 +1323,7 @@
       <c r="J23" s="14">
         <v>0.47638888888888892</v>
       </c>
-      <c r="K23" s="23">
+      <c r="K23" s="20">
         <f>INT((J23-C23)*1440)</f>
         <v>205</v>
       </c>
@@ -1418,7 +1417,7 @@
         <f t="shared" si="7"/>
         <v>9</v>
       </c>
-      <c r="K26" s="23">
+      <c r="K26" s="20">
         <f>SUM(D26:J26)</f>
         <v>2058</v>
       </c>
@@ -1450,7 +1449,7 @@
       <c r="J28" s="14">
         <v>0.51666666666666672</v>
       </c>
-      <c r="K28" s="23">
+      <c r="K28" s="20">
         <f>INT((J28-C28)*1440)</f>
         <v>262</v>
       </c>
@@ -1544,7 +1543,7 @@
         <f t="shared" ref="J31" si="25">IF(J30&lt;0, J30*-3, J30)</f>
         <v>5</v>
       </c>
-      <c r="K31" s="23">
+      <c r="K31" s="20">
         <f>SUM(D31:J31)</f>
         <v>2110</v>
       </c>
@@ -1572,7 +1571,7 @@
       <c r="H33" s="14"/>
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
-      <c r="K33" s="23">
+      <c r="K33" s="20">
         <f t="shared" ref="K33" si="26">INT((J33-C33)*1440)</f>
         <v>-523</v>
       </c>
@@ -1666,7 +1665,7 @@
         <f t="shared" si="35"/>
         <v>90</v>
       </c>
-      <c r="K36" s="23">
+      <c r="K36" s="20">
         <f t="shared" ref="K36" si="36">SUM(D36:J36)</f>
         <v>2602</v>
       </c>
@@ -1686,7 +1685,7 @@
       <c r="H38" s="17"/>
       <c r="I38" s="17"/>
       <c r="J38" s="17"/>
-      <c r="K38" s="24">
+      <c r="K38" s="21">
         <f t="shared" ref="K38" si="37">INT((J38-C38)*1440)</f>
         <v>0</v>
       </c>
@@ -1791,7 +1790,7 @@
         <f t="shared" si="46"/>
         <v>90</v>
       </c>
-      <c r="K41" s="24">
+      <c r="K41" s="21">
         <f t="shared" ref="K41" si="47">SUM(D41:J41)</f>
         <v>462</v>
       </c>
@@ -1821,7 +1820,7 @@
       <c r="J43" s="14">
         <v>0.50277777777777777</v>
       </c>
-      <c r="K43" s="23">
+      <c r="K43" s="20">
         <f t="shared" ref="K43" si="48">INT((J43-C43)*1440)</f>
         <v>238</v>
       </c>
@@ -1915,7 +1914,7 @@
         <f t="shared" si="57"/>
         <v>11</v>
       </c>
-      <c r="K46" s="23">
+      <c r="K46" s="20">
         <f t="shared" ref="K46" si="58">SUM(D46:J46)</f>
         <v>5059</v>
       </c>
@@ -1949,7 +1948,7 @@
       <c r="J48" s="14">
         <v>0.51041666666666663</v>
       </c>
-      <c r="K48" s="23">
+      <c r="K48" s="20">
         <f t="shared" ref="K48" si="59">INT((J48-C48)*1440)</f>
         <v>248</v>
       </c>
@@ -2043,7 +2042,7 @@
         <f t="shared" si="46"/>
         <v>30</v>
       </c>
-      <c r="K51" s="23">
+      <c r="K51" s="20">
         <f t="shared" ref="K51" si="69">SUM(D51:J51)</f>
         <v>2153</v>
       </c>
@@ -2065,7 +2064,7 @@
       <c r="H53" s="17"/>
       <c r="I53" s="17"/>
       <c r="J53" s="17"/>
-      <c r="K53" s="24">
+      <c r="K53" s="21">
         <f t="shared" ref="K53" si="70">INT((J53-C53)*1440)</f>
         <v>0</v>
       </c>
@@ -2170,7 +2169,7 @@
         <f t="shared" si="79"/>
         <v>90</v>
       </c>
-      <c r="K56" s="24">
+      <c r="K56" s="21">
         <f t="shared" ref="K56" si="80">SUM(D56:J56)</f>
         <v>462</v>
       </c>
@@ -2200,7 +2199,7 @@
       <c r="J58" s="14">
         <v>0.4909722222222222</v>
       </c>
-      <c r="K58" s="23">
+      <c r="K58" s="20">
         <f t="shared" ref="K58" si="81">INT((J58-C58)*1440)</f>
         <v>219</v>
       </c>
@@ -2294,7 +2293,7 @@
         <f t="shared" si="46"/>
         <v>677</v>
       </c>
-      <c r="K61" s="23">
+      <c r="K61" s="20">
         <f t="shared" ref="K61" si="91">SUM(D61:J61)</f>
         <v>4889</v>
       </c>
@@ -2324,7 +2323,7 @@
       <c r="J63" s="14">
         <v>0.49027777777777781</v>
       </c>
-      <c r="K63" s="23">
+      <c r="K63" s="20">
         <f t="shared" ref="K63" si="92">INT((J63-C63)*1440)</f>
         <v>217</v>
       </c>
@@ -2418,7 +2417,7 @@
         <f t="shared" si="101"/>
         <v>676</v>
       </c>
-      <c r="K66" s="23">
+      <c r="K66" s="20">
         <f t="shared" ref="K66" si="102">SUM(D66:J66)</f>
         <v>2778</v>
       </c>
@@ -2448,7 +2447,7 @@
       </c>
       <c r="I68" s="14"/>
       <c r="J68" s="14"/>
-      <c r="K68" s="23">
+      <c r="K68" s="20">
         <f t="shared" ref="K68" si="103">INT((J68-C68)*1440)</f>
         <v>-490</v>
       </c>
@@ -2542,7 +2541,7 @@
         <f t="shared" si="46"/>
         <v>90</v>
       </c>
-      <c r="K71" s="23">
+      <c r="K71" s="20">
         <f t="shared" ref="K71" si="113">SUM(D71:J71)</f>
         <v>2111</v>
       </c>
@@ -2576,7 +2575,7 @@
       <c r="J73" s="14">
         <v>0.4777777777777778</v>
       </c>
-      <c r="K73" s="23">
+      <c r="K73" s="20">
         <f t="shared" ref="K73" si="114">INT((J73-C73)*1440)</f>
         <v>176</v>
       </c>
@@ -2670,7 +2669,7 @@
         <f t="shared" si="123"/>
         <v>1</v>
       </c>
-      <c r="K76" s="23">
+      <c r="K76" s="20">
         <f t="shared" ref="K76" si="124">SUM(D76:J76)</f>
         <v>36</v>
       </c>
@@ -2694,7 +2693,7 @@
       <c r="J78" s="14">
         <v>0.50416666666666665</v>
       </c>
-      <c r="K78" s="23">
+      <c r="K78" s="20">
         <f t="shared" ref="K78" si="125">INT((J78-C78)*1440)</f>
         <v>234</v>
       </c>
@@ -2788,7 +2787,7 @@
         <f t="shared" si="46"/>
         <v>696</v>
       </c>
-      <c r="K81" s="23">
+      <c r="K81" s="20">
         <f t="shared" ref="K81" si="135">SUM(D81:J81)</f>
         <v>4952</v>
       </c>
@@ -2822,7 +2821,7 @@
       <c r="J83" s="14">
         <v>0.50486111111111109</v>
       </c>
-      <c r="K83" s="23">
+      <c r="K83" s="20">
         <f t="shared" ref="K83" si="136">INT((J83-C83)*1440)</f>
         <v>234</v>
       </c>
@@ -2916,7 +2915,7 @@
         <f t="shared" si="145"/>
         <v>6</v>
       </c>
-      <c r="K86" s="23">
+      <c r="K86" s="20">
         <f t="shared" ref="K86" si="146">SUM(D86:J86)</f>
         <v>87</v>
       </c>
@@ -2950,7 +2949,7 @@
       <c r="J88" s="14">
         <v>0.48888888888888887</v>
       </c>
-      <c r="K88" s="23">
+      <c r="K88" s="20">
         <f t="shared" ref="K88" si="147">INT((J88-C88)*1440)</f>
         <v>164</v>
       </c>
@@ -3044,7 +3043,7 @@
         <f t="shared" si="46"/>
         <v>1</v>
       </c>
-      <c r="K91" s="23">
+      <c r="K91" s="20">
         <f t="shared" ref="K91" si="157">SUM(D91:J91)</f>
         <v>34</v>
       </c>
@@ -3074,7 +3073,7 @@
       <c r="J93" s="14">
         <v>0.52361111111111114</v>
       </c>
-      <c r="K93" s="23">
+      <c r="K93" s="20">
         <f t="shared" ref="K93" si="158">INT((J93-C93)*1440)</f>
         <v>259</v>
       </c>
@@ -3168,7 +3167,7 @@
         <f t="shared" si="167"/>
         <v>9</v>
       </c>
-      <c r="K96" s="23">
+      <c r="K96" s="20">
         <f t="shared" ref="K96" si="168">SUM(D96:J96)</f>
         <v>4885</v>
       </c>
@@ -3200,7 +3199,7 @@
       <c r="J98" s="14">
         <v>0.51111111111111118</v>
       </c>
-      <c r="K98" s="23">
+      <c r="K98" s="20">
         <f t="shared" ref="K98" si="169">INT((J98-C98)*1440)</f>
         <v>240</v>
       </c>
@@ -3294,7 +3293,7 @@
         <f t="shared" si="46"/>
         <v>9</v>
       </c>
-      <c r="K101" s="23">
+      <c r="K101" s="20">
         <f t="shared" ref="K101" si="179">SUM(D101:J101)</f>
         <v>2173</v>
       </c>
@@ -3328,7 +3327,7 @@
       <c r="J103" s="14">
         <v>0.52777777777777779</v>
       </c>
-      <c r="K103" s="23">
+      <c r="K103" s="20">
         <f t="shared" ref="K103" si="180">INT((J103-C103)*1440)</f>
         <v>235</v>
       </c>
@@ -3422,7 +3421,7 @@
         <f t="shared" si="189"/>
         <v>6</v>
       </c>
-      <c r="K106" s="23">
+      <c r="K106" s="20">
         <f t="shared" ref="K106" si="190">SUM(D106:J106)</f>
         <v>240</v>
       </c>
@@ -3456,7 +3455,7 @@
       <c r="J108" s="14">
         <v>0.5131944444444444</v>
       </c>
-      <c r="K108" s="23">
+      <c r="K108" s="20">
         <f t="shared" ref="K108" si="191">INT((J108-C108)*1440)</f>
         <v>241</v>
       </c>
@@ -3550,7 +3549,7 @@
         <f t="shared" si="200"/>
         <v>24</v>
       </c>
-      <c r="K111" s="23">
+      <c r="K111" s="20">
         <f t="shared" ref="K111" si="201">SUM(D111:J111)</f>
         <v>85</v>
       </c>
@@ -3578,7 +3577,7 @@
       <c r="J113" s="14">
         <v>0.4909722222222222</v>
       </c>
-      <c r="K113" s="23">
+      <c r="K113" s="20">
         <f t="shared" ref="K113" si="202">INT((J113-C113)*1440)</f>
         <v>207</v>
       </c>
@@ -3672,7 +3671,7 @@
         <f t="shared" si="211"/>
         <v>677</v>
       </c>
-      <c r="K116" s="23">
+      <c r="K116" s="20">
         <f t="shared" ref="K116" si="212">SUM(D116:J116)</f>
         <v>4764</v>
       </c>
@@ -3702,7 +3701,7 @@
       <c r="J118" s="14">
         <v>0.51041666666666663</v>
       </c>
-      <c r="K118" s="23">
+      <c r="K118" s="20">
         <f t="shared" ref="K118" si="213">INT((J118-C118)*1440)</f>
         <v>234</v>
       </c>
@@ -3796,7 +3795,7 @@
         <f t="shared" si="200"/>
         <v>30</v>
       </c>
-      <c r="K121" s="23">
+      <c r="K121" s="20">
         <f t="shared" ref="K121" si="223">SUM(D121:J121)</f>
         <v>4843</v>
       </c>
@@ -3828,7 +3827,7 @@
       <c r="J123" s="14">
         <v>0.55694444444444446</v>
       </c>
-      <c r="K123" s="23">
+      <c r="K123" s="20">
         <f t="shared" ref="K123" si="224">INT((J123-C123)*1440)</f>
         <v>269</v>
       </c>
@@ -3922,7 +3921,7 @@
         <f t="shared" si="233"/>
         <v>1</v>
       </c>
-      <c r="K126" s="23">
+      <c r="K126" s="20">
         <f t="shared" ref="K126" si="234">SUM(D126:J126)</f>
         <v>2318</v>
       </c>
@@ -3952,7 +3951,7 @@
         <v>0.47222222222222227</v>
       </c>
       <c r="J128" s="14"/>
-      <c r="K128" s="23">
+      <c r="K128" s="20">
         <f t="shared" ref="K128" si="235">INT((J128-C128)*1440)</f>
         <v>-502</v>
       </c>
@@ -4046,7 +4045,7 @@
         <f t="shared" si="200"/>
         <v>2130</v>
       </c>
-      <c r="K131" s="23">
+      <c r="K131" s="20">
         <f t="shared" ref="K131" si="245">SUM(D131:J131)</f>
         <v>4454</v>
       </c>
@@ -4076,7 +4075,7 @@
       <c r="J133" s="15">
         <v>0.48333333333333334</v>
       </c>
-      <c r="K133" s="25">
+      <c r="K133" s="22">
         <f t="shared" ref="K133" si="246">INT((J133-C133)*1440)</f>
         <v>193</v>
       </c>
@@ -4170,7 +4169,7 @@
         <f t="shared" si="255"/>
         <v>9</v>
       </c>
-      <c r="K136" s="23">
+      <c r="K136" s="20">
         <f t="shared" ref="K136" si="256">SUM(D136:J136)</f>
         <v>2935</v>
       </c>
@@ -4190,7 +4189,7 @@
       <c r="H138" s="17"/>
       <c r="I138" s="17"/>
       <c r="J138" s="17"/>
-      <c r="K138" s="24">
+      <c r="K138" s="21">
         <f t="shared" ref="K138" si="257">INT((J138-C138)*1440)</f>
         <v>0</v>
       </c>
@@ -4295,7 +4294,7 @@
         <f t="shared" si="200"/>
         <v>90</v>
       </c>
-      <c r="K141" s="24">
+      <c r="K141" s="21">
         <f t="shared" ref="K141" si="267">SUM(D141:J141)</f>
         <v>462</v>
       </c>
@@ -4327,7 +4326,7 @@
       <c r="J143" s="14">
         <v>0.50416666666666665</v>
       </c>
-      <c r="K143" s="23">
+      <c r="K143" s="20">
         <f t="shared" ref="K143" si="268">INT((J143-C143)*1440)</f>
         <v>206</v>
       </c>
@@ -4421,7 +4420,7 @@
         <f t="shared" si="277"/>
         <v>3</v>
       </c>
-      <c r="K146" s="23">
+      <c r="K146" s="20">
         <f t="shared" ref="K146" si="278">SUM(D146:J146)</f>
         <v>2223</v>
       </c>
@@ -4451,7 +4450,7 @@
       <c r="J148" s="14">
         <v>0.51041666666666663</v>
       </c>
-      <c r="K148" s="23">
+      <c r="K148" s="20">
         <f t="shared" ref="K148" si="279">INT((J148-C148)*1440)</f>
         <v>229</v>
       </c>
@@ -4545,7 +4544,7 @@
         <f t="shared" si="200"/>
         <v>3</v>
       </c>
-      <c r="K151" s="23">
+      <c r="K151" s="20">
         <f t="shared" ref="K151" si="289">SUM(D151:J151)</f>
         <v>4891</v>
       </c>
@@ -4579,7 +4578,7 @@
       <c r="J153" s="15">
         <v>0.47986111111111113</v>
       </c>
-      <c r="K153" s="25">
+      <c r="K153" s="22">
         <f t="shared" ref="K153" si="290">INT((J153-C153)*1440)</f>
         <v>184</v>
       </c>
@@ -4673,7 +4672,7 @@
         <f t="shared" si="299"/>
         <v>9</v>
       </c>
-      <c r="K156" s="23">
+      <c r="K156" s="20">
         <f t="shared" ref="K156" si="300">SUM(D156:J156)</f>
         <v>53</v>
       </c>
@@ -4707,7 +4706,7 @@
       <c r="J158" s="14">
         <v>0.49583333333333335</v>
       </c>
-      <c r="K158" s="23">
+      <c r="K158" s="20">
         <f t="shared" ref="K158" si="301">INT((J158-C158)*1440)</f>
         <v>206</v>
       </c>
@@ -4801,7 +4800,7 @@
         <f t="shared" si="200"/>
         <v>684</v>
       </c>
-      <c r="K161" s="23">
+      <c r="K161" s="20">
         <f t="shared" ref="K161" si="310">SUM(D161:J161)</f>
         <v>2831</v>
       </c>
@@ -4823,7 +4822,7 @@
       <c r="H163" s="17"/>
       <c r="I163" s="17"/>
       <c r="J163" s="17"/>
-      <c r="K163" s="24">
+      <c r="K163" s="21">
         <f t="shared" ref="K163" si="311">INT((J163-C163)*1440)</f>
         <v>0</v>
       </c>
@@ -4928,7 +4927,7 @@
         <f t="shared" si="320"/>
         <v>90</v>
       </c>
-      <c r="K166" s="24">
+      <c r="K166" s="21">
         <f t="shared" ref="K166" si="321">SUM(D166:J166)</f>
         <v>462</v>
       </c>
@@ -4962,7 +4961,7 @@
       <c r="J168" s="14">
         <v>0.47013888888888888</v>
       </c>
-      <c r="K168" s="23">
+      <c r="K168" s="20">
         <f t="shared" ref="K168" si="322">INT((J168-C168)*1440)</f>
         <v>167</v>
       </c>
@@ -5056,7 +5055,7 @@
         <f t="shared" si="200"/>
         <v>0</v>
       </c>
-      <c r="K171" s="23">
+      <c r="K171" s="20">
         <f t="shared" ref="K171" si="332">SUM(D171:J171)</f>
         <v>27</v>
       </c>
@@ -5090,7 +5089,7 @@
       <c r="J173" s="14">
         <v>0.50486111111111109</v>
       </c>
-      <c r="K173" s="23">
+      <c r="K173" s="20">
         <f t="shared" ref="K173" si="333">INT((J173-C173)*1440)</f>
         <v>216</v>
       </c>
@@ -5184,7 +5183,7 @@
         <f t="shared" si="342"/>
         <v>2</v>
       </c>
-      <c r="K176" s="23">
+      <c r="K176" s="20">
         <f t="shared" ref="K176" si="343">SUM(D176:J176)</f>
         <v>61</v>
       </c>
@@ -5214,7 +5213,7 @@
       <c r="J178" s="17">
         <v>0.55486111111111114</v>
       </c>
-      <c r="K178" s="24">
+      <c r="K178" s="21">
         <f t="shared" ref="K178" si="344">INT((J178-C178)*1440)</f>
         <v>799</v>
       </c>
@@ -5319,7 +5318,7 @@
         <f t="shared" si="353"/>
         <v>3</v>
       </c>
-      <c r="K181" s="24">
+      <c r="K181" s="21">
         <f t="shared" ref="K181" si="354">SUM(D181:J181)</f>
         <v>876</v>
       </c>
@@ -5345,7 +5344,7 @@
       <c r="H183" s="14"/>
       <c r="I183" s="14"/>
       <c r="J183" s="14"/>
-      <c r="K183" s="23">
+      <c r="K183" s="20">
         <f t="shared" ref="K183" si="355">INT((J183-C183)*1440)</f>
         <v>-513</v>
       </c>
@@ -5439,7 +5438,7 @@
         <f t="shared" si="364"/>
         <v>90</v>
       </c>
-      <c r="K186" s="23">
+      <c r="K186" s="20">
         <f t="shared" ref="K186" si="365">SUM(D186:J186)</f>
         <v>4656</v>
       </c>
@@ -5471,7 +5470,7 @@
       <c r="J188" s="14">
         <v>0.48680555555555555</v>
       </c>
-      <c r="K188" s="23">
+      <c r="K188" s="20">
         <f t="shared" ref="K188" si="366">INT((J188-C188)*1440)</f>
         <v>187</v>
       </c>
@@ -5565,7 +5564,7 @@
         <f t="shared" si="353"/>
         <v>7</v>
       </c>
-      <c r="K191" s="23">
+      <c r="K191" s="20">
         <f t="shared" ref="K191" si="376">SUM(D191:J191)</f>
         <v>2640</v>
       </c>
@@ -5593,7 +5592,7 @@
       <c r="H193" s="15"/>
       <c r="I193" s="15"/>
       <c r="J193" s="15"/>
-      <c r="K193" s="25">
+      <c r="K193" s="22">
         <f t="shared" ref="K193" si="377">INT((J193-C193)*1440)</f>
         <v>-515</v>
       </c>
@@ -5687,7 +5686,7 @@
         <f t="shared" si="386"/>
         <v>90</v>
       </c>
-      <c r="K196" s="23">
+      <c r="K196" s="20">
         <f t="shared" ref="K196" si="387">SUM(D196:J196)</f>
         <v>2913</v>
       </c>
@@ -5721,7 +5720,7 @@
       <c r="J198" s="14">
         <v>0.51250000000000007</v>
       </c>
-      <c r="K198" s="23">
+      <c r="K198" s="20">
         <f t="shared" ref="K198" si="388">INT((J198-C198)*1440)</f>
         <v>222</v>
       </c>
@@ -5815,7 +5814,7 @@
         <f t="shared" si="353"/>
         <v>18</v>
       </c>
-      <c r="K201" s="23">
+      <c r="K201" s="20">
         <f t="shared" ref="K201" si="398">SUM(D201:J201)</f>
         <v>90</v>
       </c>
@@ -5849,7 +5848,7 @@
       <c r="J203" s="14">
         <v>0.49513888888888885</v>
       </c>
-      <c r="K203" s="23">
+      <c r="K203" s="20">
         <f t="shared" ref="K203" si="399">INT((J203-C203)*1440)</f>
         <v>196</v>
       </c>
@@ -5943,7 +5942,7 @@
         <f t="shared" si="408"/>
         <v>4</v>
       </c>
-      <c r="K206" s="23">
+      <c r="K206" s="20">
         <f t="shared" ref="K206" si="409">SUM(D206:J206)</f>
         <v>45</v>
       </c>
@@ -5973,7 +5972,7 @@
       <c r="J208" s="14">
         <v>0.49513888888888885</v>
       </c>
-      <c r="K208" s="23">
+      <c r="K208" s="20">
         <f t="shared" ref="K208" si="410">INT((J208-C208)*1440)</f>
         <v>195</v>
       </c>
@@ -6067,7 +6066,7 @@
         <f t="shared" si="353"/>
         <v>4</v>
       </c>
-      <c r="K211" s="23">
+      <c r="K211" s="20">
         <f t="shared" ref="K211" si="420">SUM(D211:J211)</f>
         <v>4865</v>
       </c>
@@ -6095,7 +6094,7 @@
       <c r="J213" s="17">
         <v>0.54791666666666672</v>
       </c>
-      <c r="K213" s="24">
+      <c r="K213" s="21">
         <f t="shared" ref="K213" si="421">INT((J213-C213)*1440)</f>
         <v>789</v>
       </c>
@@ -6200,7 +6199,7 @@
         <f t="shared" si="430"/>
         <v>3</v>
       </c>
-      <c r="K216" s="24">
+      <c r="K216" s="21">
         <f t="shared" ref="K216" si="431">SUM(D216:J216)</f>
         <v>914</v>
       </c>
@@ -6232,7 +6231,7 @@
       <c r="J218" s="14">
         <v>0.51736111111111105</v>
       </c>
-      <c r="K218" s="23">
+      <c r="K218" s="20">
         <f t="shared" ref="K218" si="432">INT((J218-C218)*1440)</f>
         <v>225</v>
       </c>
@@ -6326,7 +6325,7 @@
         <f t="shared" si="441"/>
         <v>21</v>
       </c>
-      <c r="K221" s="23">
+      <c r="K221" s="20">
         <f t="shared" ref="K221" si="442">SUM(D221:J221)</f>
         <v>2841</v>
       </c>
@@ -6360,7 +6359,7 @@
       <c r="J223" s="14">
         <v>0.51736111111111105</v>
       </c>
-      <c r="K223" s="23">
+      <c r="K223" s="20">
         <f t="shared" ref="K223" si="443">INT((J223-C223)*1440)</f>
         <v>224</v>
       </c>
@@ -6454,7 +6453,7 @@
         <f t="shared" si="452"/>
         <v>24</v>
       </c>
-      <c r="K226" s="23">
+      <c r="K226" s="20">
         <f t="shared" ref="K226" si="453">SUM(D226:J226)</f>
         <v>101</v>
       </c>
@@ -6482,7 +6481,7 @@
       <c r="J228" s="17">
         <v>0.55486111111111114</v>
       </c>
-      <c r="K228" s="24">
+      <c r="K228" s="21">
         <f t="shared" ref="K228" si="454">INT((J228-C228)*1440)</f>
         <v>799</v>
       </c>
@@ -6587,7 +6586,7 @@
         <f t="shared" si="441"/>
         <v>3</v>
       </c>
-      <c r="K231" s="24">
+      <c r="K231" s="21">
         <f t="shared" ref="K231" si="464">SUM(D231:J231)</f>
         <v>876</v>
       </c>
@@ -6619,7 +6618,7 @@
       <c r="J233" s="14">
         <v>0.50902777777777775</v>
       </c>
-      <c r="K233" s="23">
+      <c r="K233" s="20">
         <f t="shared" ref="K233" si="465">INT((J233-C233)*1440)</f>
         <v>209</v>
       </c>
@@ -6713,7 +6712,7 @@
         <f t="shared" si="474"/>
         <v>1</v>
       </c>
-      <c r="K236" s="23">
+      <c r="K236" s="20">
         <f t="shared" ref="K236" si="475">SUM(D236:J236)</f>
         <v>2735</v>
       </c>
@@ -6743,7 +6742,7 @@
       <c r="J238" s="17">
         <v>0.55486111111111114</v>
       </c>
-      <c r="K238" s="24">
+      <c r="K238" s="21">
         <f t="shared" ref="K238" si="476">INT((J238-C238)*1440)</f>
         <v>799</v>
       </c>
@@ -6848,7 +6847,7 @@
         <f t="shared" si="441"/>
         <v>3</v>
       </c>
-      <c r="K241" s="24">
+      <c r="K241" s="21">
         <f t="shared" ref="K241" si="486">SUM(D241:J241)</f>
         <v>2988</v>
       </c>
@@ -6882,7 +6881,7 @@
       <c r="J243" s="14">
         <v>0.47986111111111113</v>
       </c>
-      <c r="K243" s="23">
+      <c r="K243" s="20">
         <f t="shared" ref="K243" si="487">INT((J243-C243)*1440)</f>
         <v>165</v>
       </c>
@@ -6976,7 +6975,7 @@
         <f t="shared" si="496"/>
         <v>48</v>
       </c>
-      <c r="K246" s="23">
+      <c r="K246" s="20">
         <f t="shared" ref="K246" si="497">SUM(D246:J246)</f>
         <v>88</v>
       </c>
@@ -7010,7 +7009,7 @@
       <c r="J248" s="14">
         <v>0.4826388888888889</v>
       </c>
-      <c r="K248" s="23">
+      <c r="K248" s="20">
         <f t="shared" ref="K248" si="498">INT((J248-C248)*1440)</f>
         <v>168</v>
       </c>
@@ -7104,7 +7103,7 @@
         <f t="shared" si="441"/>
         <v>2</v>
       </c>
-      <c r="K251" s="23">
+      <c r="K251" s="20">
         <f t="shared" ref="K251" si="508">SUM(D251:J251)</f>
         <v>33</v>
       </c>
@@ -7138,7 +7137,7 @@
       <c r="J253" s="14">
         <v>0.52361111111111114</v>
       </c>
-      <c r="K253" s="23">
+      <c r="K253" s="20">
         <f t="shared" ref="K253" si="509">INT((J253-C253)*1440)</f>
         <v>226</v>
       </c>
@@ -7232,7 +7231,7 @@
         <f t="shared" si="518"/>
         <v>18</v>
       </c>
-      <c r="K256" s="23">
+      <c r="K256" s="20">
         <f t="shared" ref="K256" si="519">SUM(D256:J256)</f>
         <v>98</v>
       </c>
@@ -7266,7 +7265,7 @@
       <c r="J258" s="14">
         <v>0.51041666666666663</v>
       </c>
-      <c r="K258" s="23">
+      <c r="K258" s="20">
         <f t="shared" ref="K258" si="520">INT((J258-C258)*1440)</f>
         <v>206</v>
       </c>
@@ -7360,7 +7359,7 @@
         <f t="shared" si="529"/>
         <v>8</v>
       </c>
-      <c r="K261" s="23">
+      <c r="K261" s="20">
         <f t="shared" ref="K261" si="530">SUM(D261:J261)</f>
         <v>59</v>
       </c>
@@ -7390,7 +7389,7 @@
         <v>0.53472222222222221</v>
       </c>
       <c r="J263" s="14"/>
-      <c r="K263" s="23">
+      <c r="K263" s="20">
         <f t="shared" ref="K263" si="531">INT((J263-C263)*1440)</f>
         <v>-530</v>
       </c>
@@ -7484,7 +7483,7 @@
         <f t="shared" si="540"/>
         <v>2400</v>
       </c>
-      <c r="K266" s="23">
+      <c r="K266" s="20">
         <f t="shared" ref="K266" si="541">SUM(D266:J266)</f>
         <v>4719</v>
       </c>
@@ -7512,7 +7511,7 @@
       <c r="H268" s="14"/>
       <c r="I268" s="14"/>
       <c r="J268" s="14"/>
-      <c r="K268" s="23">
+      <c r="K268" s="20">
         <f t="shared" ref="K268" si="542">INT((J268-C268)*1440)</f>
         <v>-531</v>
       </c>
@@ -7606,7 +7605,7 @@
         <f t="shared" si="529"/>
         <v>90</v>
       </c>
-      <c r="K271" s="23">
+      <c r="K271" s="20">
         <f t="shared" ref="K271" si="552">SUM(D271:J271)</f>
         <v>2547</v>
       </c>
@@ -7638,7 +7637,7 @@
       <c r="J273" s="14">
         <v>0.49374999999999997</v>
       </c>
-      <c r="K273" s="23">
+      <c r="K273" s="20">
         <f t="shared" ref="K273" si="553">INT((J273-C273)*1440)</f>
         <v>179</v>
       </c>
@@ -7732,7 +7731,7 @@
         <f t="shared" si="562"/>
         <v>0</v>
       </c>
-      <c r="K276" s="23">
+      <c r="K276" s="20">
         <f t="shared" ref="K276" si="563">SUM(D276:J276)</f>
         <v>2704</v>
       </c>
@@ -7766,7 +7765,7 @@
       <c r="J278" s="14">
         <v>0.49236111111111108</v>
       </c>
-      <c r="K278" s="23">
+      <c r="K278" s="20">
         <f t="shared" ref="K278" si="564">INT((J278-C278)*1440)</f>
         <v>162</v>
       </c>
@@ -7860,7 +7859,7 @@
         <f t="shared" si="529"/>
         <v>0</v>
       </c>
-      <c r="K281" s="23">
+      <c r="K281" s="20">
         <f t="shared" ref="K281" si="574">SUM(D281:J281)</f>
         <v>6</v>
       </c>
@@ -7886,7 +7885,7 @@
       <c r="H283" s="14"/>
       <c r="I283" s="14"/>
       <c r="J283" s="14"/>
-      <c r="K283" s="23">
+      <c r="K283" s="20">
         <f t="shared" ref="K283" si="575">INT((J283-C283)*1440)</f>
         <v>-534</v>
       </c>
@@ -7980,7 +7979,7 @@
         <f t="shared" si="584"/>
         <v>90</v>
       </c>
-      <c r="K286" s="23">
+      <c r="K286" s="20">
         <f t="shared" ref="K286" si="585">SUM(D286:J286)</f>
         <v>4720</v>
       </c>
@@ -8014,7 +8013,7 @@
       <c r="J288" s="14">
         <v>0.5083333333333333</v>
       </c>
-      <c r="K288" s="23">
+      <c r="K288" s="20">
         <f t="shared" ref="K288" si="586">INT((J288-C288)*1440)</f>
         <v>197</v>
       </c>
@@ -8108,7 +8107,7 @@
         <f t="shared" si="529"/>
         <v>7</v>
       </c>
-      <c r="K291" s="23">
+      <c r="K291" s="20">
         <f t="shared" ref="K291" si="596">SUM(D291:J291)</f>
         <v>42</v>
       </c>
@@ -8142,7 +8141,7 @@
       <c r="J293" s="14">
         <v>0.51527777777777783</v>
       </c>
-      <c r="K293" s="23">
+      <c r="K293" s="20">
         <f t="shared" ref="K293" si="597">INT((J293-C293)*1440)</f>
         <v>206</v>
       </c>
@@ -8236,7 +8235,7 @@
         <f t="shared" si="606"/>
         <v>2</v>
       </c>
-      <c r="K296" s="23">
+      <c r="K296" s="20">
         <f t="shared" ref="K296" si="607">SUM(D296:J296)</f>
         <v>64</v>
       </c>
@@ -8264,7 +8263,7 @@
       <c r="J298" s="14">
         <v>0.55486111111111114</v>
       </c>
-      <c r="K298" s="23">
+      <c r="K298" s="20">
         <f t="shared" ref="K298" si="608">INT((J298-C298)*1440)</f>
         <v>262</v>
       </c>
@@ -8358,7 +8357,7 @@
         <f t="shared" si="617"/>
         <v>3</v>
       </c>
-      <c r="K301" s="23">
+      <c r="K301" s="20">
         <f t="shared" ref="K301" si="618">SUM(D301:J301)</f>
         <v>7724</v>
       </c>
@@ -8386,7 +8385,7 @@
       <c r="J303" s="14">
         <v>0.54791666666666672</v>
       </c>
-      <c r="K303" s="23">
+      <c r="K303" s="20">
         <f t="shared" ref="K303" si="619">INT((J303-C303)*1440)</f>
         <v>251</v>
       </c>
@@ -8480,7 +8479,7 @@
         <f t="shared" si="628"/>
         <v>3</v>
       </c>
-      <c r="K306" s="23">
+      <c r="K306" s="20">
         <f t="shared" ref="K306" si="629">SUM(D306:J306)</f>
         <v>8093</v>
       </c>
@@ -8510,7 +8509,7 @@
       <c r="J308" s="14">
         <v>0.55486111111111114</v>
       </c>
-      <c r="K308" s="23">
+      <c r="K308" s="20">
         <f t="shared" ref="K308" si="630">INT((J308-C308)*1440)</f>
         <v>260</v>
       </c>
@@ -8604,7 +8603,7 @@
         <f t="shared" si="617"/>
         <v>3</v>
       </c>
-      <c r="K311" s="23">
+      <c r="K311" s="20">
         <f t="shared" ref="K311" si="640">SUM(D311:J311)</f>
         <v>5357</v>
       </c>
@@ -8632,7 +8631,7 @@
       <c r="J313" s="14">
         <v>0.54791666666666672</v>
       </c>
-      <c r="K313" s="23">
+      <c r="K313" s="20">
         <f t="shared" ref="K313" si="641">INT((J313-C313)*1440)</f>
         <v>789</v>
       </c>
@@ -8726,7 +8725,7 @@
         <f t="shared" ref="J316" si="662">IF(J315&lt;0, J315*-3, J315)</f>
         <v>3</v>
       </c>
-      <c r="K316" s="23">
+      <c r="K316" s="20">
         <f t="shared" ref="K316" si="663">SUM(D316:J316)</f>
         <v>6479</v>
       </c>
@@ -8756,7 +8755,7 @@
       <c r="J318" s="14">
         <v>0.55486111111111114</v>
       </c>
-      <c r="K318" s="23">
+      <c r="K318" s="20">
         <f t="shared" ref="K318" si="664">INT((J318-C318)*1440)</f>
         <v>258</v>
       </c>
@@ -8850,7 +8849,7 @@
         <f t="shared" ref="J321" si="685">IF(J320&lt;0, J320*-3, J320)</f>
         <v>3</v>
       </c>
-      <c r="K321" s="23">
+      <c r="K321" s="20">
         <f t="shared" ref="K321" si="686">SUM(D321:J321)</f>
         <v>5779</v>
       </c>
@@ -8884,7 +8883,7 @@
       <c r="J323" s="15">
         <v>0.54791666666666672</v>
       </c>
-      <c r="K323" s="25">
+      <c r="K323" s="22">
         <f t="shared" ref="K323" si="687">INT((J323-C323)*1440)</f>
         <v>247</v>
       </c>
@@ -8978,7 +8977,7 @@
         <f t="shared" ref="J326" si="708">IF(J325&lt;0, J325*-3, J325)</f>
         <v>6</v>
       </c>
-      <c r="K326" s="23">
+      <c r="K326" s="20">
         <f t="shared" ref="K326" si="709">SUM(D326:J326)</f>
         <v>99</v>
       </c>
@@ -9008,7 +9007,7 @@
       <c r="J328" s="17">
         <v>0.55486111111111114</v>
       </c>
-      <c r="K328" s="24">
+      <c r="K328" s="21">
         <f t="shared" ref="K328" si="710">INT((J328-C328)*1440)</f>
         <v>799</v>
       </c>
@@ -9113,7 +9112,7 @@
         <f t="shared" ref="J331" si="731">IF(J330&lt;0, J330*-3, J330)</f>
         <v>3</v>
       </c>
-      <c r="K331" s="24">
+      <c r="K331" s="21">
         <f t="shared" ref="K331" si="732">SUM(D331:J331)</f>
         <v>3673</v>
       </c>
@@ -9158,7 +9157,7 @@
       <c r="J333" s="17">
         <v>0.54791666666666672</v>
       </c>
-      <c r="K333" s="24">
+      <c r="K333" s="21">
         <f t="shared" ref="K333" si="733">INT((J333-C333)*1440)</f>
         <v>789</v>
       </c>
@@ -9263,7 +9262,7 @@
         <f t="shared" ref="J336" si="754">IF(J335&lt;0, J335*-3, J335)</f>
         <v>3</v>
       </c>
-      <c r="K336" s="24">
+      <c r="K336" s="21">
         <f t="shared" ref="K336" si="755">SUM(D336:J336)</f>
         <v>762</v>
       </c>
@@ -9310,7 +9309,7 @@
       <c r="J338" s="17">
         <v>0.55486111111111114</v>
       </c>
-      <c r="K338" s="24">
+      <c r="K338" s="21">
         <f t="shared" ref="K338" si="756">INT((J338-C338)*1440)</f>
         <v>799</v>
       </c>
@@ -9415,7 +9414,7 @@
         <f t="shared" ref="J341" si="777">IF(J340&lt;0, J340*-3, J340)</f>
         <v>3</v>
       </c>
-      <c r="K341" s="24">
+      <c r="K341" s="21">
         <f t="shared" ref="K341" si="778">SUM(D341:J341)</f>
         <v>716</v>
       </c>
@@ -9447,7 +9446,7 @@
       <c r="J343" s="14">
         <v>0.54166666666666663</v>
       </c>
-      <c r="K343" s="23">
+      <c r="K343" s="20">
         <f t="shared" ref="K343" si="779">INT((J343-C343)*1440)</f>
         <v>234</v>
       </c>
@@ -9541,7 +9540,7 @@
         <f t="shared" ref="J346" si="800">IF(J345&lt;0, J345*-3, J345)</f>
         <v>45</v>
       </c>
-      <c r="K346" s="23">
+      <c r="K346" s="20">
         <f t="shared" ref="K346" si="801">SUM(D346:J346)</f>
         <v>3166</v>
       </c>
@@ -9575,7 +9574,7 @@
       <c r="J348" s="17">
         <v>0.55486111111111114</v>
       </c>
-      <c r="K348" s="24">
+      <c r="K348" s="21">
         <f t="shared" ref="K348" si="802">INT((J348-C348)*1440)</f>
         <v>799</v>
       </c>
@@ -9680,7 +9679,7 @@
         <f t="shared" ref="J351" si="823">IF(J350&lt;0, J350*-3, J350)</f>
         <v>3</v>
       </c>
-      <c r="K351" s="24">
+      <c r="K351" s="21">
         <f t="shared" ref="K351" si="824">SUM(D351:J351)</f>
         <v>716</v>
       </c>
@@ -9727,7 +9726,7 @@
       <c r="J353" s="17">
         <v>0.54791666666666672</v>
       </c>
-      <c r="K353" s="24">
+      <c r="K353" s="21">
         <f t="shared" ref="K353" si="825">INT((J353-C353)*1440)</f>
         <v>789</v>
       </c>
@@ -9832,7 +9831,7 @@
         <f t="shared" ref="J356" si="846">IF(J355&lt;0, J355*-3, J355)</f>
         <v>3</v>
       </c>
-      <c r="K356" s="24">
+      <c r="K356" s="21">
         <f t="shared" ref="K356" si="847">SUM(D356:J356)</f>
         <v>762</v>
       </c>
@@ -9879,7 +9878,7 @@
       <c r="J358" s="17">
         <v>0.55486111111111114</v>
       </c>
-      <c r="K358" s="24">
+      <c r="K358" s="21">
         <f t="shared" ref="K358" si="848">INT((J358-C358)*1440)</f>
         <v>799</v>
       </c>
@@ -9984,7 +9983,7 @@
         <f t="shared" ref="J361" si="869">IF(J360&lt;0, J360*-3, J360)</f>
         <v>3</v>
       </c>
-      <c r="K361" s="24">
+      <c r="K361" s="21">
         <f t="shared" ref="K361" si="870">SUM(D361:J361)</f>
         <v>716</v>
       </c>
@@ -10031,7 +10030,7 @@
       <c r="J363" s="17">
         <v>0.54791666666666672</v>
       </c>
-      <c r="K363" s="24">
+      <c r="K363" s="21">
         <f t="shared" ref="K363" si="871">INT((J363-C363)*1440)</f>
         <v>789</v>
       </c>
@@ -10136,7 +10135,7 @@
         <f t="shared" ref="J366" si="892">IF(J365&lt;0, J365*-3, J365)</f>
         <v>3</v>
       </c>
-      <c r="K366" s="24">
+      <c r="K366" s="21">
         <f t="shared" ref="K366" si="893">SUM(D366:J366)</f>
         <v>762</v>
       </c>
@@ -10175,7 +10174,7 @@
       <c r="J368" s="14">
         <v>0.54166666666666663</v>
       </c>
-      <c r="K368" s="23">
+      <c r="K368" s="20">
         <f t="shared" ref="K368" si="894">INT((J368-C368)*1440)</f>
         <v>235</v>
       </c>
@@ -10269,7 +10268,7 @@
         <f t="shared" ref="J371" si="915">IF(J370&lt;0, J370*-3, J370)</f>
         <v>42</v>
       </c>
-      <c r="K371" s="23">
+      <c r="K371" s="20">
         <f t="shared" ref="K371" si="916">SUM(D371:J371)</f>
         <v>177</v>
       </c>
@@ -10303,7 +10302,7 @@
       <c r="J373" s="15">
         <v>0.52361111111111114</v>
       </c>
-      <c r="K373" s="25">
+      <c r="K373" s="22">
         <f t="shared" ref="K373" si="917">INT((J373-C373)*1440)</f>
         <v>211</v>
       </c>
@@ -10397,7 +10396,7 @@
         <f t="shared" ref="J376" si="938">IF(J375&lt;0, J375*-3, J375)</f>
         <v>18</v>
       </c>
-      <c r="K376" s="23">
+      <c r="K376" s="20">
         <f t="shared" ref="K376" si="939">SUM(D376:J376)</f>
         <v>108</v>
       </c>
@@ -10431,7 +10430,7 @@
       <c r="J378" s="14">
         <v>0.55486111111111114</v>
       </c>
-      <c r="K378" s="23">
+      <c r="K378" s="20">
         <f t="shared" ref="K378" si="940">INT((J378-C378)*1440)</f>
         <v>255</v>
       </c>
@@ -10525,13 +10524,12 @@
         <f t="shared" ref="J381" si="961">IF(J380&lt;0, J380*-3, J380)</f>
         <v>32</v>
       </c>
-      <c r="K381" s="23">
+      <c r="K381" s="20">
         <f t="shared" ref="K381" si="962">SUM(D381:J381)</f>
         <v>180</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A20:K382" xr:uid="{F5A2BD83-87CC-4D86-B37D-1F1B84049F58}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
@@ -10545,7 +10543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEBFBA6-03F8-4558-9AFD-35C4CA5D21E7}">
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -10581,1872 +10579,1872 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="26">
+      <c r="A2" s="23">
         <v>1</v>
       </c>
-      <c r="B2" s="27">
+      <c r="B2" s="24">
         <v>0.33402777777777781</v>
       </c>
       <c r="C2" s="14"/>
-      <c r="D2" s="27">
+      <c r="D2" s="24">
         <v>0.36388888888888887</v>
       </c>
-      <c r="E2" s="27">
+      <c r="E2" s="24">
         <v>0.38055555555555554</v>
       </c>
-      <c r="F2" s="27">
+      <c r="F2" s="24">
         <v>0.41388888888888892</v>
       </c>
-      <c r="G2" s="27">
+      <c r="G2" s="24">
         <v>0.4368055555555555</v>
       </c>
-      <c r="H2" s="27">
+      <c r="H2" s="24">
         <v>0.45763888888888887</v>
       </c>
-      <c r="I2" s="27">
+      <c r="I2" s="24">
         <v>0.47638888888888892</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="26">
+      <c r="A3" s="23">
         <v>2</v>
       </c>
-      <c r="B3" s="27">
+      <c r="B3" s="24">
         <v>0.3347222222222222</v>
       </c>
       <c r="C3" s="14"/>
-      <c r="D3" s="27">
+      <c r="D3" s="24">
         <v>0.38055555555555554</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="24">
         <v>0.43611111111111112</v>
       </c>
-      <c r="F3" s="27">
+      <c r="F3" s="24">
         <v>0.46249999999999997</v>
       </c>
-      <c r="G3" s="27">
+      <c r="G3" s="24">
         <v>0.48055555555555557</v>
       </c>
-      <c r="H3" s="27">
+      <c r="H3" s="24">
         <v>0.49236111111111108</v>
       </c>
-      <c r="I3" s="27">
+      <c r="I3" s="24">
         <v>0.51666666666666672</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="26">
+      <c r="A4" s="23">
         <v>3</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B4" s="24">
         <v>0.36319444444444443</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="24">
         <v>0.43124999999999997</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="24">
         <v>0.45763888888888887</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="24">
         <v>0.48749999999999999</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="24">
         <v>0.52013888888888882</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="26">
+      <c r="A5" s="23">
         <v>4</v>
       </c>
-      <c r="B5" s="27">
-        <v>0</v>
-      </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
+      <c r="B5" s="24">
+        <v>0</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+      <c r="A6" s="23">
         <v>5</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="24">
         <v>0.33749999999999997</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="24">
         <v>0.37083333333333335</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="24">
         <v>0.38819444444444445</v>
       </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27">
+      <c r="E6" s="24"/>
+      <c r="F6" s="24">
         <v>0.44236111111111115</v>
       </c>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27">
+      <c r="G6" s="24"/>
+      <c r="H6" s="24">
         <v>0.47361111111111115</v>
       </c>
-      <c r="I6" s="27">
+      <c r="I6" s="24">
         <v>0.50277777777777777</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="26">
+      <c r="A7" s="23">
         <v>6</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="24">
         <v>0.33819444444444446</v>
       </c>
-      <c r="C7" s="27">
-        <v>0</v>
-      </c>
-      <c r="D7" s="27">
+      <c r="C7" s="24">
+        <v>0</v>
+      </c>
+      <c r="D7" s="24">
         <v>0.3833333333333333</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="24">
         <v>0.41875000000000001</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="24">
         <v>0.44791666666666669</v>
       </c>
-      <c r="G7" s="27">
+      <c r="G7" s="24">
         <v>0.48055555555555557</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7" s="24">
         <v>0.49583333333333335</v>
       </c>
-      <c r="I7" s="27">
+      <c r="I7" s="24">
         <v>0.51041666666666663</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="26">
+      <c r="A8" s="23">
         <v>7</v>
       </c>
-      <c r="B8" s="27">
-        <v>0</v>
-      </c>
-      <c r="C8" s="27">
-        <v>0</v>
-      </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
+      <c r="B8" s="24">
+        <v>0</v>
+      </c>
+      <c r="C8" s="24">
+        <v>0</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="25">
         <v>0.33888888888888885</v>
       </c>
-      <c r="C9" s="29">
-        <v>0</v>
-      </c>
-      <c r="D9" s="29">
+      <c r="C9" s="25">
+        <v>0</v>
+      </c>
+      <c r="D9" s="25">
         <v>0.3923611111111111</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="25">
         <v>0.42499999999999999</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="25">
         <v>0.45763888888888887</v>
       </c>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29">
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25">
         <v>0.4909722222222222</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="28">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="25">
         <v>0.33958333333333335</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="25">
         <v>0.36944444444444446</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="25">
         <v>0.38472222222222219</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="25">
         <v>0.41875000000000001</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="25">
         <v>0.44305555555555554</v>
       </c>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29">
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25">
         <v>0.49027777777777781</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="28">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="25">
         <v>0.34027777777777773</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="25">
         <v>0.36944444444444446</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="25">
         <v>0.3833333333333333</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="25">
         <v>0.39583333333333331</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="25">
         <v>0.42708333333333331</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="25">
         <v>0.44375000000000003</v>
       </c>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="28">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="29">
+      <c r="B12" s="25">
         <v>0.35555555555555557</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="25">
         <v>0.37291666666666662</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12" s="25">
         <v>0.38680555555555557</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E12" s="25">
         <v>0.40277777777777773</v>
       </c>
-      <c r="F12" s="29">
+      <c r="F12" s="25">
         <v>0.42291666666666666</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12" s="25">
         <v>0.43888888888888888</v>
       </c>
-      <c r="H12" s="29">
+      <c r="H12" s="25">
         <v>0.45624999999999999</v>
       </c>
-      <c r="I12" s="29">
+      <c r="I12" s="25">
         <v>0.4777777777777778</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="28">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="29">
+      <c r="B13" s="25">
         <v>0.34166666666666662</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29">
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25">
         <v>0.43263888888888885</v>
       </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29">
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25">
         <v>0.50416666666666665</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="28">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="29">
+      <c r="B14" s="25">
         <v>0.34236111111111112</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="25">
         <v>0.36944444444444446</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="25">
         <v>0.38472222222222219</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="25">
         <v>0.41805555555555557</v>
       </c>
-      <c r="F14" s="29">
+      <c r="F14" s="25">
         <v>0.44166666666666665</v>
       </c>
-      <c r="G14" s="29">
+      <c r="G14" s="25">
         <v>0.46597222222222223</v>
       </c>
-      <c r="H14" s="29">
+      <c r="H14" s="25">
         <v>0.48541666666666666</v>
       </c>
-      <c r="I14" s="29">
+      <c r="I14" s="25">
         <v>0.50486111111111109</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="28">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="29">
+      <c r="B15" s="25">
         <v>0.375</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="25">
         <v>0.39583333333333331</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="25">
         <v>0.40625</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="25">
         <v>0.42083333333333334</v>
       </c>
-      <c r="F15" s="29">
+      <c r="F15" s="25">
         <v>0.44027777777777777</v>
       </c>
-      <c r="G15" s="29">
+      <c r="G15" s="25">
         <v>0.45763888888888887</v>
       </c>
-      <c r="H15" s="29">
+      <c r="H15" s="25">
         <v>0.46736111111111112</v>
       </c>
-      <c r="I15" s="29">
+      <c r="I15" s="25">
         <v>0.48888888888888887</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="28">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="29">
+      <c r="B16" s="25">
         <v>0.34375</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29">
+      <c r="C16" s="25"/>
+      <c r="D16" s="25">
         <v>0.38680555555555557</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="25">
         <v>0.4201388888888889</v>
       </c>
-      <c r="F16" s="29">
+      <c r="F16" s="25">
         <v>0.4548611111111111</v>
       </c>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29">
+      <c r="G16" s="25"/>
+      <c r="H16" s="25">
         <v>0.49652777777777773</v>
       </c>
-      <c r="I16" s="29">
+      <c r="I16" s="25">
         <v>0.52361111111111114</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="28">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="29">
+      <c r="B17" s="25">
         <v>0.3444444444444445</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29">
+      <c r="C17" s="25"/>
+      <c r="D17" s="25">
         <v>0.40763888888888888</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E17" s="25">
         <v>0.42638888888888887</v>
       </c>
-      <c r="F17" s="29">
+      <c r="F17" s="25">
         <v>0.46249999999999997</v>
       </c>
-      <c r="G17" s="29">
+      <c r="G17" s="25">
         <v>0.48541666666666666</v>
       </c>
-      <c r="H17" s="29">
+      <c r="H17" s="25">
         <v>0.49236111111111108</v>
       </c>
-      <c r="I17" s="29">
+      <c r="I17" s="25">
         <v>0.51111111111111118</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="28">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="29">
+      <c r="B18" s="25">
         <v>0.36458333333333331</v>
       </c>
-      <c r="C18" s="29">
+      <c r="C18" s="25">
         <v>0.38194444444444442</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D18" s="25">
         <v>0.4145833333333333</v>
       </c>
-      <c r="E18" s="29">
+      <c r="E18" s="25">
         <v>0.45069444444444445</v>
       </c>
-      <c r="F18" s="29">
+      <c r="F18" s="25">
         <v>0.48402777777777778</v>
       </c>
-      <c r="G18" s="29">
+      <c r="G18" s="25">
         <v>0.47638888888888892</v>
       </c>
-      <c r="H18" s="29">
+      <c r="H18" s="25">
         <v>0.5083333333333333</v>
       </c>
-      <c r="I18" s="29">
+      <c r="I18" s="25">
         <v>0.52777777777777779</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="28">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="25">
         <v>0.34583333333333338</v>
       </c>
-      <c r="C19" s="29">
+      <c r="C19" s="25">
         <v>0.37013888888888885</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D19" s="25">
         <v>0.3888888888888889</v>
       </c>
-      <c r="E19" s="29">
+      <c r="E19" s="25">
         <v>0.41041666666666665</v>
       </c>
-      <c r="F19" s="29">
+      <c r="F19" s="25">
         <v>0.44236111111111115</v>
       </c>
-      <c r="G19" s="29">
+      <c r="G19" s="25">
         <v>0.46458333333333335</v>
       </c>
-      <c r="H19" s="29">
+      <c r="H19" s="25">
         <v>0.47569444444444442</v>
       </c>
-      <c r="I19" s="29">
+      <c r="I19" s="25">
         <v>0.5131944444444444</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="28">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="29">
+      <c r="B20" s="25">
         <v>0.34722222222222227</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29">
+      <c r="C20" s="25"/>
+      <c r="D20" s="25">
         <v>0.38194444444444442</v>
       </c>
-      <c r="E20" s="29">
+      <c r="E20" s="25">
         <v>0.39652777777777781</v>
       </c>
-      <c r="F20" s="29">
+      <c r="F20" s="25">
         <v>0.42986111111111108</v>
       </c>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29">
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25">
         <v>0.4909722222222222</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="28">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="29">
+      <c r="B21" s="25">
         <v>0.34791666666666665</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29">
+      <c r="C21" s="25"/>
+      <c r="D21" s="25">
         <v>0.39097222222222222</v>
       </c>
-      <c r="E21" s="29">
+      <c r="E21" s="25">
         <v>0.41041666666666665</v>
       </c>
-      <c r="F21" s="29">
+      <c r="F21" s="25">
         <v>0.44097222222222227</v>
       </c>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29">
+      <c r="G21" s="25"/>
+      <c r="H21" s="25">
         <v>0.49583333333333335</v>
       </c>
-      <c r="I21" s="29">
+      <c r="I21" s="25">
         <v>0.51041666666666663</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="28">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="29">
+      <c r="B22" s="25">
         <v>0.37013888888888885</v>
       </c>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29">
+      <c r="C22" s="25"/>
+      <c r="D22" s="25">
         <v>0.43333333333333335</v>
       </c>
-      <c r="E22" s="29">
+      <c r="E22" s="25">
         <v>0.46319444444444446</v>
       </c>
-      <c r="F22" s="29">
+      <c r="F22" s="25">
         <v>0.50277777777777777</v>
       </c>
-      <c r="G22" s="29">
+      <c r="G22" s="25">
         <v>0.52500000000000002</v>
       </c>
-      <c r="H22" s="29">
+      <c r="H22" s="25">
         <v>0.53541666666666665</v>
       </c>
-      <c r="I22" s="29">
+      <c r="I22" s="25">
         <v>0.55694444444444446</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="28">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="29">
+      <c r="B23" s="25">
         <v>0.34861111111111115</v>
       </c>
-      <c r="C23" s="29">
+      <c r="C23" s="25">
         <v>0.36388888888888887</v>
       </c>
-      <c r="D23" s="29">
+      <c r="D23" s="25">
         <v>0.37777777777777777</v>
       </c>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29">
+      <c r="E23" s="25"/>
+      <c r="F23" s="25">
         <v>0.41944444444444445</v>
       </c>
-      <c r="G23" s="29">
+      <c r="G23" s="25">
         <v>0.4368055555555555</v>
       </c>
-      <c r="H23" s="29">
+      <c r="H23" s="25">
         <v>0.47222222222222227</v>
       </c>
-      <c r="I23" s="29"/>
+      <c r="I23" s="25"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="28">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="29">
+      <c r="B24" s="25">
         <v>0.34930555555555554</v>
       </c>
-      <c r="C24" s="29">
+      <c r="C24" s="25">
         <v>0.36805555555555558</v>
       </c>
-      <c r="D24" s="29">
+      <c r="D24" s="25">
         <v>0.45</v>
       </c>
-      <c r="E24" s="29">
+      <c r="E24" s="25">
         <v>0.41388888888888892</v>
       </c>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29">
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25">
         <v>0.46458333333333335</v>
       </c>
-      <c r="I24" s="29">
+      <c r="I24" s="25">
         <v>0.48333333333333334</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="28">
+      <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="29">
-        <v>0</v>
-      </c>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
+      <c r="B25" s="25">
+        <v>0</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="28">
+      <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="29">
+      <c r="B26" s="25">
         <v>0.3611111111111111</v>
       </c>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29">
+      <c r="C26" s="25"/>
+      <c r="D26" s="25">
         <v>0.40486111111111112</v>
       </c>
-      <c r="E26" s="29">
+      <c r="E26" s="25">
         <v>0.42152777777777778</v>
       </c>
-      <c r="F26" s="29">
+      <c r="F26" s="25">
         <v>0.44861111111111113</v>
       </c>
-      <c r="G26" s="29">
+      <c r="G26" s="25">
         <v>0.4770833333333333</v>
       </c>
-      <c r="H26" s="29">
+      <c r="H26" s="25">
         <v>0.48402777777777778</v>
       </c>
-      <c r="I26" s="29">
+      <c r="I26" s="25">
         <v>0.50416666666666665</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="28">
+      <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="29">
+      <c r="B27" s="25">
         <v>0.35138888888888892</v>
       </c>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29">
+      <c r="C27" s="25"/>
+      <c r="D27" s="25">
         <v>0.39097222222222222</v>
       </c>
-      <c r="E27" s="29">
+      <c r="E27" s="25">
         <v>0.42569444444444443</v>
       </c>
-      <c r="F27" s="29">
+      <c r="F27" s="25">
         <v>0.45347222222222222</v>
       </c>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29">
+      <c r="G27" s="25"/>
+      <c r="H27" s="25">
         <v>0.48749999999999999</v>
       </c>
-      <c r="I27" s="29">
+      <c r="I27" s="25">
         <v>0.51041666666666663</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="28">
+      <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="29">
+      <c r="B28" s="25">
         <v>0.3520833333333333</v>
       </c>
-      <c r="C28" s="29">
+      <c r="C28" s="25">
         <v>0.37291666666666662</v>
       </c>
-      <c r="D28" s="29">
+      <c r="D28" s="25">
         <v>0.38750000000000001</v>
       </c>
-      <c r="E28" s="29">
+      <c r="E28" s="25">
         <v>0.4069444444444445</v>
       </c>
-      <c r="F28" s="29">
+      <c r="F28" s="25">
         <v>0.43333333333333335</v>
       </c>
-      <c r="G28" s="29">
+      <c r="G28" s="25">
         <v>0.45347222222222222</v>
       </c>
-      <c r="H28" s="29">
+      <c r="H28" s="25">
         <v>0.46111111111111108</v>
       </c>
-      <c r="I28" s="29">
+      <c r="I28" s="25">
         <v>0.47986111111111113</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="28">
+      <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="29">
+      <c r="B29" s="25">
         <v>0.3527777777777778</v>
       </c>
-      <c r="C29" s="29">
+      <c r="C29" s="25">
         <v>0.36736111111111108</v>
       </c>
-      <c r="D29" s="29">
+      <c r="D29" s="25">
         <v>0.3840277777777778</v>
       </c>
-      <c r="E29" s="29">
+      <c r="E29" s="25">
         <v>0.42499999999999999</v>
       </c>
-      <c r="F29" s="29">
+      <c r="F29" s="25">
         <v>0.45208333333333334</v>
       </c>
-      <c r="G29" s="29">
+      <c r="G29" s="25">
         <v>0.47291666666666665</v>
       </c>
-      <c r="H29" s="29">
-        <v>0</v>
-      </c>
-      <c r="I29" s="29">
+      <c r="H29" s="25">
+        <v>0</v>
+      </c>
+      <c r="I29" s="25">
         <v>0.49583333333333335</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="28">
+      <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="29">
-        <v>0</v>
-      </c>
-      <c r="C30" s="29">
-        <v>0</v>
-      </c>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
+      <c r="B30" s="25">
+        <v>0</v>
+      </c>
+      <c r="C30" s="25">
+        <v>0</v>
+      </c>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="25"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="28">
+      <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="29">
+      <c r="B31" s="25">
         <v>0.35416666666666669</v>
       </c>
-      <c r="C31" s="29">
+      <c r="C31" s="25">
         <v>0.36736111111111108</v>
       </c>
-      <c r="D31" s="29">
+      <c r="D31" s="25">
         <v>0.38055555555555554</v>
       </c>
-      <c r="E31" s="29">
+      <c r="E31" s="25">
         <v>0.3979166666666667</v>
       </c>
-      <c r="F31" s="29">
+      <c r="F31" s="25">
         <v>0.4201388888888889</v>
       </c>
-      <c r="G31" s="29">
+      <c r="G31" s="25">
         <v>0.4368055555555555</v>
       </c>
-      <c r="H31" s="29">
+      <c r="H31" s="25">
         <v>0.44930555555555557</v>
       </c>
-      <c r="I31" s="29">
+      <c r="I31" s="25">
         <v>0.47013888888888888</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="28">
+      <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="29">
+      <c r="B32" s="25">
         <v>0.35486111111111113</v>
       </c>
-      <c r="C32" s="29">
+      <c r="C32" s="25">
         <v>0.37291666666666662</v>
       </c>
-      <c r="D32" s="29">
+      <c r="D32" s="25">
         <v>0.3972222222222222</v>
       </c>
-      <c r="E32" s="29">
+      <c r="E32" s="25">
         <v>0.41944444444444445</v>
       </c>
-      <c r="F32" s="29">
+      <c r="F32" s="25">
         <v>0.45</v>
       </c>
-      <c r="G32" s="29">
+      <c r="G32" s="25">
         <v>0.47291666666666665</v>
       </c>
-      <c r="H32" s="29">
+      <c r="H32" s="25">
         <v>0.4826388888888889</v>
       </c>
-      <c r="I32" s="29">
+      <c r="I32" s="25">
         <v>0.50486111111111109</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="28">
+      <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="29">
-        <v>0</v>
-      </c>
-      <c r="C33" s="29">
-        <v>0</v>
-      </c>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29">
+      <c r="B33" s="25">
+        <v>0</v>
+      </c>
+      <c r="C33" s="25">
+        <v>0</v>
+      </c>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25">
         <v>0.49444444444444446</v>
       </c>
-      <c r="G33" s="29">
+      <c r="G33" s="25">
         <v>0.51944444444444449</v>
       </c>
-      <c r="H33" s="29">
+      <c r="H33" s="25">
         <v>0.53194444444444444</v>
       </c>
-      <c r="I33" s="29">
+      <c r="I33" s="25">
         <v>0.55486111111111114</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="28">
+      <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="29">
+      <c r="B34" s="25">
         <v>0.35625000000000001</v>
       </c>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29">
+      <c r="C34" s="25"/>
+      <c r="D34" s="25">
         <v>0.40625</v>
       </c>
-      <c r="E34" s="29">
+      <c r="E34" s="25">
         <v>0.45902777777777781</v>
       </c>
-      <c r="F34" s="29">
+      <c r="F34" s="25">
         <v>0.50624999999999998</v>
       </c>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="29"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="28">
+      <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="29">
+      <c r="B35" s="25">
         <v>0.35694444444444445</v>
       </c>
-      <c r="C35" s="29">
+      <c r="C35" s="25">
         <v>0.37083333333333335</v>
       </c>
-      <c r="D35" s="29">
+      <c r="D35" s="25">
         <v>0.38750000000000001</v>
       </c>
-      <c r="E35" s="29">
+      <c r="E35" s="25">
         <v>0.40416666666666662</v>
       </c>
-      <c r="F35" s="29">
+      <c r="F35" s="25">
         <v>0.43402777777777773</v>
       </c>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29">
+      <c r="G35" s="25"/>
+      <c r="H35" s="25">
         <v>0.46111111111111108</v>
       </c>
-      <c r="I35" s="29">
+      <c r="I35" s="25">
         <v>0.48680555555555555</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="28">
+      <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="29">
+      <c r="B36" s="25">
         <v>0.3576388888888889</v>
       </c>
-      <c r="C36" s="29">
+      <c r="C36" s="25">
         <v>0.40416666666666662</v>
       </c>
-      <c r="D36" s="29">
+      <c r="D36" s="25">
         <v>0.44236111111111115</v>
       </c>
-      <c r="E36" s="29">
+      <c r="E36" s="25">
         <v>0.4055555555555555</v>
       </c>
-      <c r="F36" s="29">
+      <c r="F36" s="25">
         <v>0.52083333333333337</v>
       </c>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="29"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="28">
+      <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="29">
+      <c r="B37" s="25">
         <v>0.35833333333333334</v>
       </c>
-      <c r="C37" s="29">
+      <c r="C37" s="25">
         <v>0.37291666666666662</v>
       </c>
-      <c r="D37" s="29">
+      <c r="D37" s="25">
         <v>0.38819444444444445</v>
       </c>
-      <c r="E37" s="29">
+      <c r="E37" s="25">
         <v>0.4055555555555555</v>
       </c>
-      <c r="F37" s="29">
+      <c r="F37" s="25">
         <v>0.43541666666666662</v>
       </c>
-      <c r="G37" s="29">
+      <c r="G37" s="25">
         <v>0.48125000000000001</v>
       </c>
-      <c r="H37" s="29">
+      <c r="H37" s="25">
         <v>0.49583333333333335</v>
       </c>
-      <c r="I37" s="29">
+      <c r="I37" s="25">
         <v>0.51250000000000007</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="28">
+      <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="29">
+      <c r="B38" s="25">
         <v>0.35902777777777778</v>
       </c>
-      <c r="C38" s="29">
+      <c r="C38" s="25">
         <v>0.37361111111111112</v>
       </c>
-      <c r="D38" s="29">
+      <c r="D38" s="25">
         <v>0.39027777777777778</v>
       </c>
-      <c r="E38" s="29">
+      <c r="E38" s="25">
         <v>0.40902777777777777</v>
       </c>
-      <c r="F38" s="29">
+      <c r="F38" s="25">
         <v>0.44166666666666665</v>
       </c>
-      <c r="G38" s="29">
+      <c r="G38" s="25">
         <v>0.46180555555555558</v>
       </c>
-      <c r="H38" s="29">
+      <c r="H38" s="25">
         <v>0.47083333333333338</v>
       </c>
-      <c r="I38" s="29">
+      <c r="I38" s="25">
         <v>0.49513888888888885</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="28">
+      <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="29">
+      <c r="B39" s="25">
         <v>0.35972222222222222</v>
       </c>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29">
+      <c r="C39" s="25"/>
+      <c r="D39" s="25">
         <v>0.39097222222222222</v>
       </c>
-      <c r="E39" s="29">
+      <c r="E39" s="25">
         <v>0.40972222222222227</v>
       </c>
-      <c r="F39" s="29">
+      <c r="F39" s="25">
         <v>0.4465277777777778</v>
       </c>
-      <c r="G39" s="29"/>
-      <c r="H39" s="29">
+      <c r="G39" s="25"/>
+      <c r="H39" s="25">
         <v>0.47152777777777777</v>
       </c>
-      <c r="I39" s="29">
+      <c r="I39" s="25">
         <v>0.49513888888888885</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="28">
+      <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="29">
-        <v>0</v>
-      </c>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29">
+      <c r="B40" s="25">
+        <v>0</v>
+      </c>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25">
         <v>0.50416666666666665</v>
       </c>
-      <c r="G40" s="29">
+      <c r="G40" s="25">
         <v>0.51944444444444449</v>
       </c>
-      <c r="H40" s="29">
+      <c r="H40" s="25">
         <v>0.52500000000000002</v>
       </c>
-      <c r="I40" s="29">
+      <c r="I40" s="25">
         <v>0.54791666666666672</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="28">
+      <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="29">
+      <c r="B41" s="25">
         <v>0.3611111111111111</v>
       </c>
-      <c r="C41" s="29">
+      <c r="C41" s="25">
         <v>0.38750000000000001</v>
       </c>
-      <c r="D41" s="29">
+      <c r="D41" s="25">
         <v>0.4152777777777778</v>
       </c>
-      <c r="E41" s="29">
+      <c r="E41" s="25">
         <v>0.43541666666666662</v>
       </c>
-      <c r="F41" s="29">
+      <c r="F41" s="25">
         <v>0.45763888888888887</v>
       </c>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29">
+      <c r="G41" s="25"/>
+      <c r="H41" s="25">
         <v>0.50069444444444444</v>
       </c>
-      <c r="I41" s="29">
+      <c r="I41" s="25">
         <v>0.51736111111111105</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="28">
+      <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="29">
+      <c r="B42" s="25">
         <v>0.36180555555555555</v>
       </c>
-      <c r="C42" s="29">
+      <c r="C42" s="25">
         <v>0.3833333333333333</v>
       </c>
-      <c r="D42" s="29">
+      <c r="D42" s="25">
         <v>0.40763888888888888</v>
       </c>
-      <c r="E42" s="29">
+      <c r="E42" s="25">
         <v>0.42708333333333331</v>
       </c>
-      <c r="F42" s="29">
+      <c r="F42" s="25">
         <v>0.46249999999999997</v>
       </c>
-      <c r="G42" s="29">
+      <c r="G42" s="25">
         <v>0.48333333333333334</v>
       </c>
-      <c r="H42" s="29">
+      <c r="H42" s="25">
         <v>0.50138888888888888</v>
       </c>
-      <c r="I42" s="29">
+      <c r="I42" s="25">
         <v>0.51736111111111105</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="28">
+      <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="29">
-        <v>0</v>
-      </c>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29">
+      <c r="B43" s="25">
+        <v>0</v>
+      </c>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25">
         <v>0.49444444444444446</v>
       </c>
-      <c r="G43" s="29">
+      <c r="G43" s="25">
         <v>0.51944444444444449</v>
       </c>
-      <c r="H43" s="29">
+      <c r="H43" s="25">
         <v>0.53194444444444444</v>
       </c>
-      <c r="I43" s="29">
+      <c r="I43" s="25">
         <v>0.55486111111111114</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="28">
+      <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="29">
+      <c r="B44" s="25">
         <v>0.36388888888888887</v>
       </c>
-      <c r="C44" s="29">
+      <c r="C44" s="25">
         <v>0.39513888888888887</v>
       </c>
-      <c r="D44" s="29">
+      <c r="D44" s="25">
         <v>0.41111111111111115</v>
       </c>
-      <c r="E44" s="29">
+      <c r="E44" s="25">
         <v>0.42777777777777781</v>
       </c>
-      <c r="F44" s="29">
+      <c r="F44" s="25">
         <v>0.4465277777777778</v>
       </c>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29">
+      <c r="G44" s="25"/>
+      <c r="H44" s="25">
         <v>0.48749999999999999</v>
       </c>
-      <c r="I44" s="29">
+      <c r="I44" s="25">
         <v>0.50902777777777775</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="28">
+      <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="29">
-        <v>0</v>
-      </c>
-      <c r="C45" s="29">
+      <c r="B45" s="25">
+        <v>0</v>
+      </c>
+      <c r="C45" s="25">
         <v>0.37916666666666665</v>
       </c>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29">
+      <c r="D45" s="25"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25">
         <v>0.49444444444444446</v>
       </c>
-      <c r="G45" s="29">
+      <c r="G45" s="25">
         <v>0.51944444444444449</v>
       </c>
-      <c r="H45" s="29">
+      <c r="H45" s="25">
         <v>0.53194444444444444</v>
       </c>
-      <c r="I45" s="29">
+      <c r="I45" s="25">
         <v>0.55486111111111114</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="28">
+      <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="29">
+      <c r="B46" s="25">
         <v>0.36527777777777781</v>
       </c>
-      <c r="C46" s="29">
+      <c r="C46" s="25">
         <v>0.37916666666666665</v>
       </c>
-      <c r="D46" s="29">
+      <c r="D46" s="25">
         <v>0.3972222222222222</v>
       </c>
-      <c r="E46" s="29">
+      <c r="E46" s="25">
         <v>0.4152777777777778</v>
       </c>
-      <c r="F46" s="29">
+      <c r="F46" s="25">
         <v>0.43958333333333338</v>
       </c>
-      <c r="G46" s="29">
+      <c r="G46" s="25">
         <v>0.46249999999999997</v>
       </c>
-      <c r="H46" s="29">
+      <c r="H46" s="25">
         <v>0.4694444444444445</v>
       </c>
-      <c r="I46" s="29">
+      <c r="I46" s="25">
         <v>0.47986111111111113</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="28">
+      <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="29">
+      <c r="B47" s="25">
         <v>0.3659722222222222</v>
       </c>
-      <c r="C47" s="29">
+      <c r="C47" s="25">
         <v>0.38194444444444442</v>
       </c>
-      <c r="D47" s="29">
+      <c r="D47" s="25">
         <v>0.39652777777777781</v>
       </c>
-      <c r="E47" s="29">
+      <c r="E47" s="25">
         <v>0.4152777777777778</v>
       </c>
-      <c r="F47" s="29">
+      <c r="F47" s="25">
         <v>0.43541666666666662</v>
       </c>
-      <c r="G47" s="29">
+      <c r="G47" s="25">
         <v>0.45277777777777778</v>
       </c>
-      <c r="H47" s="29">
+      <c r="H47" s="25">
         <v>0.4604166666666667</v>
       </c>
-      <c r="I47" s="29">
+      <c r="I47" s="25">
         <v>0.4826388888888889</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="28">
+      <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="29">
+      <c r="B48" s="25">
         <v>0.3666666666666667</v>
       </c>
-      <c r="C48" s="29">
+      <c r="C48" s="25">
         <v>0.37916666666666665</v>
       </c>
-      <c r="D48" s="29">
+      <c r="D48" s="25">
         <v>0.4069444444444445</v>
       </c>
-      <c r="E48" s="29">
+      <c r="E48" s="25">
         <v>0.44097222222222227</v>
       </c>
-      <c r="F48" s="29">
+      <c r="F48" s="25">
         <v>0.4680555555555555</v>
       </c>
-      <c r="G48" s="29">
+      <c r="G48" s="25">
         <v>0.4909722222222222</v>
       </c>
-      <c r="H48" s="29">
+      <c r="H48" s="25">
         <v>0.50694444444444442</v>
       </c>
-      <c r="I48" s="29">
+      <c r="I48" s="25">
         <v>0.52361111111111114</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="28">
+      <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="29">
+      <c r="B49" s="25">
         <v>0.36736111111111108</v>
       </c>
-      <c r="C49" s="29">
+      <c r="C49" s="25">
         <v>0.38472222222222219</v>
       </c>
-      <c r="D49" s="29">
+      <c r="D49" s="25">
         <v>0.4055555555555555</v>
       </c>
-      <c r="E49" s="29">
+      <c r="E49" s="25">
         <v>0.42222222222222222</v>
       </c>
-      <c r="F49" s="29">
+      <c r="F49" s="25">
         <v>0.45416666666666666</v>
       </c>
-      <c r="G49" s="29">
+      <c r="G49" s="25">
         <v>0.47152777777777777</v>
       </c>
-      <c r="H49" s="29">
+      <c r="H49" s="25">
         <v>0.48333333333333334</v>
       </c>
-      <c r="I49" s="29">
+      <c r="I49" s="25">
         <v>0.51041666666666663</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="28">
+      <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="29">
+      <c r="B50" s="25">
         <v>0.36805555555555558</v>
       </c>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29">
+      <c r="C50" s="25"/>
+      <c r="D50" s="25">
         <v>0.42083333333333334</v>
       </c>
-      <c r="E50" s="29">
+      <c r="E50" s="25">
         <v>0.4777777777777778</v>
       </c>
-      <c r="F50" s="29">
+      <c r="F50" s="25">
         <v>0.50416666666666665</v>
       </c>
-      <c r="G50" s="29">
+      <c r="G50" s="25">
         <v>0.52708333333333335</v>
       </c>
-      <c r="H50" s="29">
+      <c r="H50" s="25">
         <v>0.53472222222222221</v>
       </c>
-      <c r="I50" s="29"/>
+      <c r="I50" s="25"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="28">
+      <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" s="29">
+      <c r="B51" s="25">
         <v>0.36874999999999997</v>
       </c>
-      <c r="C51" s="29">
+      <c r="C51" s="25">
         <v>0.3972222222222222</v>
       </c>
-      <c r="D51" s="29">
+      <c r="D51" s="25">
         <v>0.42291666666666666</v>
       </c>
-      <c r="E51" s="29">
+      <c r="E51" s="25">
         <v>0.46388888888888885</v>
       </c>
-      <c r="F51" s="29">
+      <c r="F51" s="25">
         <v>0.51180555555555551</v>
       </c>
-      <c r="G51" s="29"/>
-      <c r="H51" s="29"/>
-      <c r="I51" s="29"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="25"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="28">
+      <c r="A52">
         <v>51</v>
       </c>
-      <c r="B52" s="29">
+      <c r="B52" s="25">
         <v>0.36944444444444446</v>
       </c>
-      <c r="C52" s="29">
+      <c r="C52" s="25">
         <v>0.38750000000000001</v>
       </c>
-      <c r="D52" s="29">
+      <c r="D52" s="25">
         <v>0.40486111111111112</v>
       </c>
-      <c r="E52" s="29">
+      <c r="E52" s="25">
         <v>0.42291666666666666</v>
       </c>
-      <c r="F52" s="29">
+      <c r="F52" s="25">
         <v>0.4465277777777778</v>
       </c>
-      <c r="G52" s="29"/>
-      <c r="H52" s="29">
+      <c r="G52" s="25"/>
+      <c r="H52" s="25">
         <v>0.47222222222222227</v>
       </c>
-      <c r="I52" s="29">
+      <c r="I52" s="25">
         <v>0.49374999999999997</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="28">
+      <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53" s="29">
+      <c r="B53" s="25">
         <v>0.37986111111111115</v>
       </c>
-      <c r="C53" s="29">
+      <c r="C53" s="25">
         <v>0.39374999999999999</v>
       </c>
-      <c r="D53" s="29">
+      <c r="D53" s="25">
         <v>0.4069444444444445</v>
       </c>
-      <c r="E53" s="29">
+      <c r="E53" s="25">
         <v>0.4236111111111111</v>
       </c>
-      <c r="F53" s="29">
+      <c r="F53" s="25">
         <v>0.44305555555555554</v>
       </c>
-      <c r="G53" s="29">
+      <c r="G53" s="25">
         <v>0.46180555555555558</v>
       </c>
-      <c r="H53" s="29">
+      <c r="H53" s="25">
         <v>0.47152777777777777</v>
       </c>
-      <c r="I53" s="29">
+      <c r="I53" s="25">
         <v>0.49236111111111108</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="28">
+      <c r="A54">
         <v>53</v>
       </c>
-      <c r="B54" s="29">
+      <c r="B54" s="25">
         <v>0.37083333333333335</v>
       </c>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29">
+      <c r="C54" s="25"/>
+      <c r="D54" s="25">
         <v>0.42083333333333334</v>
       </c>
-      <c r="E54" s="29">
+      <c r="E54" s="25">
         <v>0.4597222222222222</v>
       </c>
-      <c r="F54" s="29">
+      <c r="F54" s="25">
         <v>0.50624999999999998</v>
       </c>
-      <c r="G54" s="29"/>
-      <c r="H54" s="29"/>
-      <c r="I54" s="29"/>
+      <c r="G54" s="25"/>
+      <c r="H54" s="25"/>
+      <c r="I54" s="25"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="28">
+      <c r="A55">
         <v>54</v>
       </c>
-      <c r="B55" s="29">
+      <c r="B55" s="25">
         <v>0.37152777777777773</v>
       </c>
-      <c r="C55" s="29">
+      <c r="C55" s="25">
         <v>0.3923611111111111</v>
       </c>
-      <c r="D55" s="29">
+      <c r="D55" s="25">
         <v>0.40763888888888888</v>
       </c>
-      <c r="E55" s="29">
+      <c r="E55" s="25">
         <v>0.42569444444444443</v>
       </c>
-      <c r="F55" s="29">
+      <c r="F55" s="25">
         <v>0.45347222222222222</v>
       </c>
-      <c r="G55" s="29">
+      <c r="G55" s="25">
         <v>0.47222222222222227</v>
       </c>
-      <c r="H55" s="29">
+      <c r="H55" s="25">
         <v>0.4826388888888889</v>
       </c>
-      <c r="I55" s="29">
+      <c r="I55" s="25">
         <v>0.5083333333333333</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="28">
+      <c r="A56">
         <v>55</v>
       </c>
-      <c r="B56" s="29">
+      <c r="B56" s="25">
         <v>0.37222222222222223</v>
       </c>
-      <c r="C56" s="29">
+      <c r="C56" s="25">
         <v>0.39374999999999999</v>
       </c>
-      <c r="D56" s="29">
+      <c r="D56" s="25">
         <v>0.40902777777777777</v>
       </c>
-      <c r="E56" s="29">
+      <c r="E56" s="25">
         <v>0.42777777777777781</v>
       </c>
-      <c r="F56" s="29">
+      <c r="F56" s="25">
         <v>0.44930555555555557</v>
       </c>
-      <c r="G56" s="29">
+      <c r="G56" s="25">
         <v>0.48541666666666666</v>
       </c>
-      <c r="H56" s="29">
+      <c r="H56" s="25">
         <v>0.49305555555555558</v>
       </c>
-      <c r="I56" s="29">
+      <c r="I56" s="25">
         <v>0.51527777777777783</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="28">
+      <c r="A57">
         <v>56</v>
       </c>
-      <c r="B57" s="29">
+      <c r="B57" s="25">
         <v>0.37291666666666662</v>
       </c>
-      <c r="C57" s="29"/>
-      <c r="D57" s="29">
+      <c r="C57" s="25"/>
+      <c r="D57" s="25">
         <v>0.40902777777777777</v>
       </c>
-      <c r="E57" s="29"/>
-      <c r="F57" s="29">
+      <c r="E57" s="25"/>
+      <c r="F57" s="25">
         <v>0.49444444444444446</v>
       </c>
-      <c r="G57" s="29"/>
-      <c r="H57" s="29">
+      <c r="G57" s="25"/>
+      <c r="H57" s="25">
         <v>0.53194444444444444</v>
       </c>
-      <c r="I57" s="29">
+      <c r="I57" s="25">
         <v>0.55486111111111114</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="28">
+      <c r="A58">
         <v>57</v>
       </c>
-      <c r="B58" s="29">
+      <c r="B58" s="25">
         <v>0.37361111111111112</v>
       </c>
-      <c r="C58" s="29"/>
-      <c r="D58" s="29">
+      <c r="C58" s="25"/>
+      <c r="D58" s="25">
         <v>0.46458333333333335</v>
       </c>
-      <c r="E58" s="29"/>
-      <c r="F58" s="29">
+      <c r="E58" s="25"/>
+      <c r="F58" s="25">
         <v>0.50416666666666665</v>
       </c>
-      <c r="G58" s="29"/>
-      <c r="H58" s="29">
+      <c r="G58" s="25"/>
+      <c r="H58" s="25">
         <v>0.52500000000000002</v>
       </c>
-      <c r="I58" s="29">
+      <c r="I58" s="25">
         <v>0.54791666666666672</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="28">
+      <c r="A59">
         <v>58</v>
       </c>
-      <c r="B59" s="29">
+      <c r="B59" s="25">
         <v>0.3743055555555555</v>
       </c>
-      <c r="C59" s="29"/>
-      <c r="D59" s="29">
+      <c r="C59" s="25"/>
+      <c r="D59" s="25">
         <v>0.45763888888888887</v>
       </c>
-      <c r="E59" s="29">
+      <c r="E59" s="25">
         <v>0.46111111111111108</v>
       </c>
-      <c r="F59" s="29">
+      <c r="F59" s="25">
         <v>0.49444444444444446</v>
       </c>
-      <c r="G59" s="29"/>
-      <c r="H59" s="29">
+      <c r="G59" s="25"/>
+      <c r="H59" s="25">
         <v>0.53194444444444444</v>
       </c>
-      <c r="I59" s="29">
+      <c r="I59" s="25">
         <v>0.55486111111111114</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="28">
+      <c r="A60">
         <v>59</v>
       </c>
-      <c r="B60" s="29">
-        <v>0</v>
-      </c>
-      <c r="C60" s="29"/>
-      <c r="D60" s="29">
+      <c r="B60" s="25">
+        <v>0</v>
+      </c>
+      <c r="C60" s="25"/>
+      <c r="D60" s="25">
         <v>0.46458333333333335</v>
       </c>
-      <c r="E60" s="29"/>
-      <c r="F60" s="29">
+      <c r="E60" s="25"/>
+      <c r="F60" s="25">
         <v>0.50416666666666665</v>
       </c>
-      <c r="G60" s="29"/>
-      <c r="H60" s="29">
+      <c r="G60" s="25"/>
+      <c r="H60" s="25">
         <v>0.52500000000000002</v>
       </c>
-      <c r="I60" s="29">
+      <c r="I60" s="25">
         <v>0.54791666666666672</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="28">
+      <c r="A61">
         <v>60</v>
       </c>
-      <c r="B61" s="29">
+      <c r="B61" s="25">
         <v>0.3756944444444445</v>
       </c>
-      <c r="C61" s="29">
+      <c r="C61" s="25">
         <v>0.42638888888888887</v>
       </c>
-      <c r="D61" s="29">
+      <c r="D61" s="25">
         <v>0.45763888888888887</v>
       </c>
-      <c r="E61" s="29"/>
-      <c r="F61" s="29">
+      <c r="E61" s="25"/>
+      <c r="F61" s="25">
         <v>0.49444444444444446</v>
       </c>
-      <c r="G61" s="29"/>
-      <c r="H61" s="29">
+      <c r="G61" s="25"/>
+      <c r="H61" s="25">
         <v>0.53194444444444444</v>
       </c>
-      <c r="I61" s="29">
+      <c r="I61" s="25">
         <v>0.55486111111111114</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="28">
+      <c r="A62">
         <v>61</v>
       </c>
-      <c r="B62" s="29">
+      <c r="B62" s="25">
         <v>0.37638888888888888</v>
       </c>
-      <c r="C62" s="29">
+      <c r="C62" s="25">
         <v>0.40902777777777777</v>
       </c>
-      <c r="D62" s="29">
+      <c r="D62" s="25">
         <v>0.43541666666666662</v>
       </c>
-      <c r="E62" s="29">
+      <c r="E62" s="25">
         <v>0.45694444444444443</v>
       </c>
-      <c r="F62" s="29">
+      <c r="F62" s="25">
         <v>0.48888888888888887</v>
       </c>
-      <c r="G62" s="29">
+      <c r="G62" s="25">
         <v>0.51874999999999993</v>
       </c>
-      <c r="H62" s="29">
+      <c r="H62" s="25">
         <v>0.52847222222222223</v>
       </c>
-      <c r="I62" s="29">
+      <c r="I62" s="25">
         <v>0.54791666666666672</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="28">
+      <c r="A63">
         <v>62</v>
       </c>
-      <c r="B63" s="29">
-        <v>0</v>
-      </c>
-      <c r="C63" s="29"/>
-      <c r="D63" s="29">
+      <c r="B63" s="25">
+        <v>0</v>
+      </c>
+      <c r="C63" s="25"/>
+      <c r="D63" s="25">
         <v>0.45763888888888887</v>
       </c>
-      <c r="E63" s="29">
+      <c r="E63" s="25">
         <v>0.47430555555555554</v>
       </c>
-      <c r="F63" s="29">
+      <c r="F63" s="25">
         <v>0.49444444444444446</v>
       </c>
-      <c r="G63" s="29"/>
-      <c r="H63" s="29">
+      <c r="G63" s="25"/>
+      <c r="H63" s="25">
         <v>0.53194444444444444</v>
       </c>
-      <c r="I63" s="29">
+      <c r="I63" s="25">
         <v>0.55486111111111114</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="28">
+      <c r="A64">
         <v>63</v>
       </c>
-      <c r="B64" s="29">
-        <v>0</v>
-      </c>
-      <c r="C64" s="29"/>
-      <c r="D64" s="29">
+      <c r="B64" s="25">
+        <v>0</v>
+      </c>
+      <c r="C64" s="25"/>
+      <c r="D64" s="25">
         <v>0.46458333333333335</v>
       </c>
-      <c r="E64" s="29">
+      <c r="E64" s="25">
         <v>0.48819444444444443</v>
       </c>
-      <c r="F64" s="29">
+      <c r="F64" s="25">
         <v>0.50416666666666665</v>
       </c>
-      <c r="G64" s="29">
+      <c r="G64" s="25">
         <v>0.51944444444444449</v>
       </c>
-      <c r="H64" s="29">
+      <c r="H64" s="25">
         <v>0.52500000000000002</v>
       </c>
-      <c r="I64" s="29">
+      <c r="I64" s="25">
         <v>0.54791666666666672</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="28">
+      <c r="A65">
         <v>64</v>
       </c>
-      <c r="B65" s="29">
-        <v>0</v>
-      </c>
-      <c r="C65" s="29">
-        <v>0</v>
-      </c>
-      <c r="D65" s="29">
+      <c r="B65" s="25">
+        <v>0</v>
+      </c>
+      <c r="C65" s="25">
+        <v>0</v>
+      </c>
+      <c r="D65" s="25">
         <v>0.45763888888888887</v>
       </c>
-      <c r="E65" s="29">
+      <c r="E65" s="25">
         <v>0.47430555555555554</v>
       </c>
-      <c r="F65" s="29">
+      <c r="F65" s="25">
         <v>0.49444444444444446</v>
       </c>
-      <c r="G65" s="29">
+      <c r="G65" s="25">
         <v>0.51944444444444449</v>
       </c>
-      <c r="H65" s="29">
+      <c r="H65" s="25">
         <v>0.53194444444444444</v>
       </c>
-      <c r="I65" s="29">
+      <c r="I65" s="25">
         <v>0.55486111111111114</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="28">
+      <c r="A66">
         <v>65</v>
       </c>
-      <c r="B66" s="29">
+      <c r="B66" s="25">
         <v>0.37916666666666665</v>
       </c>
-      <c r="C66" s="29">
+      <c r="C66" s="25">
         <v>0.40902777777777777</v>
       </c>
-      <c r="D66" s="29">
+      <c r="D66" s="25">
         <v>0.45208333333333334</v>
       </c>
-      <c r="E66" s="29">
+      <c r="E66" s="25">
         <v>0.47986111111111113</v>
       </c>
-      <c r="F66" s="29">
+      <c r="F66" s="25">
         <v>0.50694444444444442</v>
       </c>
-      <c r="G66" s="29"/>
-      <c r="H66" s="29">
+      <c r="G66" s="25"/>
+      <c r="H66" s="25">
         <v>0.53055555555555556</v>
       </c>
-      <c r="I66" s="29">
+      <c r="I66" s="25">
         <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="28">
+      <c r="A67">
         <v>66</v>
       </c>
-      <c r="B67" s="29">
-        <v>0</v>
-      </c>
-      <c r="C67" s="29">
-        <v>0</v>
-      </c>
-      <c r="D67" s="29">
+      <c r="B67" s="25">
+        <v>0</v>
+      </c>
+      <c r="C67" s="25">
+        <v>0</v>
+      </c>
+      <c r="D67" s="25">
         <v>0.45763888888888887</v>
       </c>
-      <c r="E67" s="29">
+      <c r="E67" s="25">
         <v>0.47430555555555554</v>
       </c>
-      <c r="F67" s="29">
+      <c r="F67" s="25">
         <v>0.49444444444444446</v>
       </c>
-      <c r="G67" s="29">
+      <c r="G67" s="25">
         <v>0.51944444444444449</v>
       </c>
-      <c r="H67" s="29">
+      <c r="H67" s="25">
         <v>0.53194444444444444</v>
       </c>
-      <c r="I67" s="29">
+      <c r="I67" s="25">
         <v>0.55486111111111114</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="28">
+      <c r="A68">
         <v>67</v>
       </c>
-      <c r="B68" s="29">
-        <v>0</v>
-      </c>
-      <c r="C68" s="29">
-        <v>0</v>
-      </c>
-      <c r="D68" s="29">
+      <c r="B68" s="25">
+        <v>0</v>
+      </c>
+      <c r="C68" s="25">
+        <v>0</v>
+      </c>
+      <c r="D68" s="25">
         <v>0.46458333333333335</v>
       </c>
-      <c r="E68" s="29">
+      <c r="E68" s="25">
         <v>0.48819444444444443</v>
       </c>
-      <c r="F68" s="29">
+      <c r="F68" s="25">
         <v>0.50416666666666665</v>
       </c>
-      <c r="G68" s="29">
+      <c r="G68" s="25">
         <v>0.51944444444444449</v>
       </c>
-      <c r="H68" s="29">
+      <c r="H68" s="25">
         <v>0.52500000000000002</v>
       </c>
-      <c r="I68" s="29">
+      <c r="I68" s="25">
         <v>0.54791666666666672</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="28">
+      <c r="A69">
         <v>68</v>
       </c>
-      <c r="B69" s="29">
-        <v>0</v>
-      </c>
-      <c r="C69" s="29">
-        <v>0</v>
-      </c>
-      <c r="D69" s="29">
+      <c r="B69" s="25">
+        <v>0</v>
+      </c>
+      <c r="C69" s="25">
+        <v>0</v>
+      </c>
+      <c r="D69" s="25">
         <v>0.45763888888888887</v>
       </c>
-      <c r="E69" s="29">
+      <c r="E69" s="25">
         <v>0.47430555555555554</v>
       </c>
-      <c r="F69" s="29">
+      <c r="F69" s="25">
         <v>0.49444444444444446</v>
       </c>
-      <c r="G69" s="29">
+      <c r="G69" s="25">
         <v>0.51944444444444449</v>
       </c>
-      <c r="H69" s="29">
+      <c r="H69" s="25">
         <v>0.53194444444444444</v>
       </c>
-      <c r="I69" s="29">
+      <c r="I69" s="25">
         <v>0.55486111111111114</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="28">
+      <c r="A70">
         <v>69</v>
       </c>
-      <c r="B70" s="29">
-        <v>0</v>
-      </c>
-      <c r="C70" s="29">
-        <v>0</v>
-      </c>
-      <c r="D70" s="29">
+      <c r="B70" s="25">
+        <v>0</v>
+      </c>
+      <c r="C70" s="25">
+        <v>0</v>
+      </c>
+      <c r="D70" s="25">
         <v>0.46458333333333335</v>
       </c>
-      <c r="E70" s="29">
+      <c r="E70" s="25">
         <v>0.48819444444444443</v>
       </c>
-      <c r="F70" s="29">
+      <c r="F70" s="25">
         <v>0.50416666666666665</v>
       </c>
-      <c r="G70" s="29">
+      <c r="G70" s="25">
         <v>0.51944444444444449</v>
       </c>
-      <c r="H70" s="29">
+      <c r="H70" s="25">
         <v>0.52500000000000002</v>
       </c>
-      <c r="I70" s="29">
+      <c r="I70" s="25">
         <v>0.54791666666666672</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="28">
+      <c r="A71">
         <v>70</v>
       </c>
-      <c r="B71" s="29">
+      <c r="B71" s="25">
         <v>0.37847222222222227</v>
       </c>
-      <c r="C71" s="29">
+      <c r="C71" s="25">
         <v>0.42569444444444443</v>
       </c>
-      <c r="D71" s="29">
+      <c r="D71" s="25">
         <v>0.45069444444444445</v>
       </c>
-      <c r="E71" s="29">
+      <c r="E71" s="25">
         <v>0.47847222222222219</v>
       </c>
-      <c r="F71" s="29">
+      <c r="F71" s="25">
         <v>0.5083333333333333</v>
       </c>
-      <c r="G71" s="29">
+      <c r="G71" s="25">
         <v>0.52361111111111114</v>
       </c>
-      <c r="H71" s="29">
+      <c r="H71" s="25">
         <v>0.52986111111111112</v>
       </c>
-      <c r="I71" s="29">
+      <c r="I71" s="25">
         <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="28">
+      <c r="A72">
         <v>71</v>
       </c>
-      <c r="B72" s="29">
+      <c r="B72" s="25">
         <v>0.37708333333333338</v>
       </c>
-      <c r="C72" s="29">
+      <c r="C72" s="25">
         <v>0.41736111111111113</v>
       </c>
-      <c r="D72" s="29">
+      <c r="D72" s="25">
         <v>0.44097222222222227</v>
       </c>
-      <c r="E72" s="29">
+      <c r="E72" s="25">
         <v>0.4604166666666667</v>
       </c>
-      <c r="F72" s="29">
+      <c r="F72" s="25">
         <v>0.48055555555555557</v>
       </c>
-      <c r="G72" s="29">
+      <c r="G72" s="25">
         <v>0.49513888888888885</v>
       </c>
-      <c r="H72" s="29">
+      <c r="H72" s="25">
         <v>0.50694444444444442</v>
       </c>
-      <c r="I72" s="29">
+      <c r="I72" s="25">
         <v>0.52361111111111114</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="28">
+      <c r="A73">
         <v>72</v>
       </c>
-      <c r="B73" s="29">
+      <c r="B73" s="25">
         <v>0.37777777777777777</v>
       </c>
-      <c r="C73" s="29">
+      <c r="C73" s="25">
         <v>0.41805555555555557</v>
       </c>
-      <c r="D73" s="29">
+      <c r="D73" s="25">
         <v>0.45763888888888887</v>
       </c>
-      <c r="E73" s="29">
+      <c r="E73" s="25">
         <v>0.47916666666666669</v>
       </c>
-      <c r="F73" s="29">
+      <c r="F73" s="25">
         <v>0.49583333333333335</v>
       </c>
-      <c r="G73" s="29">
+      <c r="G73" s="25">
         <v>0.50555555555555554</v>
       </c>
-      <c r="H73" s="29">
+      <c r="H73" s="25">
         <v>0.51180555555555551</v>
       </c>
-      <c r="I73" s="29">
+      <c r="I73" s="25">
         <v>0.55486111111111114</v>
       </c>
     </row>

</xml_diff>